<commit_message>
I lied... This time it's the actual last commit
</commit_message>
<xml_diff>
--- a/ryan_excel_data.xlsx
+++ b/ryan_excel_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Structure score for correct guesses</t>
   </si>
@@ -28,6 +28,15 @@
   </si>
   <si>
     <t>Percent of the time the correct model is predicted</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t># loops</t>
+  </si>
+  <si>
+    <t># models</t>
   </si>
 </sst>
 </file>
@@ -684,6 +693,203 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># models</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$43:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># loops</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$43:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$43:$D$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>781</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>838</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>944</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>951</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>959</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="92069248"/>
+        <c:axId val="93881856"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="92069248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93881856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="93881856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="92069248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -711,6 +917,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1133,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="S40" sqref="S40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1899,7 +2135,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="5:7">
+    <row r="33" spans="1:7">
       <c r="E33">
         <v>37</v>
       </c>
@@ -1911,7 +2147,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="5:7">
+    <row r="34" spans="1:7">
       <c r="E34">
         <v>40</v>
       </c>
@@ -1923,7 +2159,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="5:7">
+    <row r="35" spans="1:7">
       <c r="E35">
         <v>41</v>
       </c>
@@ -1935,7 +2171,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="5:7">
+    <row r="36" spans="1:7">
       <c r="E36">
         <v>42</v>
       </c>
@@ -1947,7 +2183,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="5:7">
+    <row r="37" spans="1:7">
       <c r="E37">
         <v>43</v>
       </c>
@@ -1959,7 +2195,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="5:7">
+    <row r="38" spans="1:7">
       <c r="E38">
         <v>50</v>
       </c>
@@ -1971,10 +2207,155 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="5:7">
+    <row r="39" spans="1:7">
       <c r="G39">
         <f>SUM(G2:G38)</f>
         <v>4482</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>643</v>
+      </c>
+      <c r="C43">
+        <f>A43*B43</f>
+        <v>643</v>
+      </c>
+      <c r="D43">
+        <f>SUM($C43:C43)</f>
+        <v>643</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44">
+        <v>69</v>
+      </c>
+      <c r="C44">
+        <f t="shared" ref="C44:C50" si="2">A44*B44</f>
+        <v>138</v>
+      </c>
+      <c r="D44">
+        <f>SUM(C43:C44)</f>
+        <v>781</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>19</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="D45">
+        <f>SUM($C43:C45)</f>
+        <v>838</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>13</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="D46">
+        <f>SUM($C43:C46)</f>
+        <v>890</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="D47">
+        <f>SUM($C43:C47)</f>
+        <v>920</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48">
+        <v>6</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D48">
+        <f>SUM($C43:C48)</f>
+        <v>944</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49">
+        <v>7</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <f>SUM($C43:C49)</f>
+        <v>951</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>8</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <f>SUM($C43:C50)</f>
+        <v>959</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="C51">
+        <f>SUM(C43:C50)</f>
+        <v>959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>